<commit_message>
Finisher this fucking rapport
</commit_message>
<xml_diff>
--- a/Pile.xlsx
+++ b/Pile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ROG\Documents\HEIG\ISI\Labos\HEIG_ISI_Labo5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E21A42C5-E725-41E5-9B3B-FDF94E668714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C73EEC1-169D-44F7-A5B4-5609F86A56C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{79CE8F7F-07B4-404E-BAD8-BDBB9D719277}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Adresse de retour de la fonction</t>
   </si>
@@ -74,9 +74,6 @@
     <t>EBP-0x18</t>
   </si>
   <si>
-    <t>EBP-0x20</t>
-  </si>
-  <si>
     <t>EBP-0x1C</t>
   </si>
   <si>
@@ -92,18 +89,9 @@
     <t>Adresse pile absolue</t>
   </si>
   <si>
-    <t>Adresse pile relative à ESP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ESP + </t>
-  </si>
-  <si>
     <t>0xffffd658</t>
   </si>
   <si>
-    <t>0xffffd65C</t>
-  </si>
-  <si>
     <t>vote[2]</t>
   </si>
   <si>
@@ -111,6 +99,30 @@
   </si>
   <si>
     <t>vote[0]</t>
+  </si>
+  <si>
+    <t>0xffffd654</t>
+  </si>
+  <si>
+    <t>0xffffd650</t>
+  </si>
+  <si>
+    <t>0xffffd64c</t>
+  </si>
+  <si>
+    <t>0xffffd648</t>
+  </si>
+  <si>
+    <t>0xffffd644</t>
+  </si>
+  <si>
+    <t>0xffffd640</t>
+  </si>
+  <si>
+    <t>0xffffd63c</t>
+  </si>
+  <si>
+    <t>0xffffd65c</t>
   </si>
 </sst>
 </file>
@@ -167,16 +179,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,153 +504,143 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C71A802F-183E-4907-B730-8BCE464D27C2}">
-  <dimension ref="A4:E14"/>
+  <dimension ref="A4:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="A4" sqref="A4:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="D5" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B7:B14"/>
+    <mergeCell ref="B7:B13"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>